<commit_message>
La matriz debe ser potencia de 2
</commit_message>
<xml_diff>
--- a/src/ArchivosC2/MatrizGrafo.xlsx
+++ b/src/ArchivosC2/MatrizGrafo.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOG-A313-E-012\Documents\NetBeansProjects\AlgorithmDesign\src\ArchivosC2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOG-A408-E-016\Documents\NetBeansProjects\AlgorithmDesign\src\ArchivosC2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -986,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,4 +2232,227 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:T30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Multiplicacion de Matrices lee dos pgs excel.
</commit_message>
<xml_diff>
--- a/src/ArchivosC2/MatrizGrafo.xlsx
+++ b/src/ArchivosC2/MatrizGrafo.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\NetBeansProjects\AlgorithmDesign\src\ArchivosC2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D28D97-5C33-424A-916D-72372202CAAA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7217C08-547C-4742-9B13-534E770355D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -995,7 +996,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1125,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1">
         <v>17</v>
@@ -1170,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1205,7 +1206,231 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67B122DB-FAE5-423E-825A-D56B75B6C58E}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1213,12 +1438,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>